<commit_message>
documentaron:   versiono \00-Documentacion\Listado_Modulos2.xlsx "descriptivo- detalle a migrar f" siniestros_unidades status_dinero trading_conv_validacion datos_fact_pedto trans_trwAnálisis Proceso con prioridad  Se agrego hoja “Analisis Proceso con prioridad”     versionador \00-Documentacion\Listado de reportes totales.xlsx
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales.xlsx
+++ b/00-Documentacion/Listado de reportes totales.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB38851-C25D-4F38-9CE3-EC6472E959DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAEC389-EE01-4554-93BD-E448E155899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
+    <sheet name="General - Analisis" sheetId="4" r:id="rId1"/>
+    <sheet name="Analisis Proceso con prioridad" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$R$1347</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Analisis Proceso con prioridad'!$A$1:$J$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'General - Analisis'!$A$1:$R$1347</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11888" uniqueCount="1737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12064" uniqueCount="1788">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5249,13 +5251,178 @@
   </si>
   <si>
     <t>no se encontro la funcion en archivo main</t>
+  </si>
+  <si>
+    <t>Reporte</t>
+  </si>
+  <si>
+    <t>Periodicidad</t>
+  </si>
+  <si>
+    <t>Procesos principales de Bosch</t>
+  </si>
+  <si>
+    <t>Expediente aduanal</t>
+  </si>
+  <si>
+    <r>
+      <t>CORRECTO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (18 CLIENTES)</t>
+    </r>
+  </si>
+  <si>
+    <t>Anexo 24 Integration Point</t>
+  </si>
+  <si>
+    <t>Lunes a sábado del día anterior</t>
+  </si>
+  <si>
+    <t>CORRECTO</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>En Espera Por Periodicidad</t>
+  </si>
+  <si>
+    <t>Interfaces SEG Automotive</t>
+  </si>
+  <si>
+    <t>El primer día del mes</t>
+  </si>
+  <si>
+    <t>Transmision COVES/EDOCs</t>
+  </si>
+  <si>
+    <t>Tiempos de despacho (Customs Clearance Times)</t>
+  </si>
+  <si>
+    <t>DAF empresa 29 mxn – de Facturación</t>
+  </si>
+  <si>
+    <t>Lunes a Sábado del día anterior</t>
+  </si>
+  <si>
+    <t>DAF fondo fijo empresa 29 mxn – de Facturación</t>
+  </si>
+  <si>
+    <t>Backlog aduana – COEX</t>
+  </si>
+  <si>
+    <t>De Lunes a Viernes</t>
+  </si>
+  <si>
+    <t>INCOMPLETO (14/15 NOTIF.)</t>
+  </si>
+  <si>
+    <t>Indices de calidad - COEX</t>
+  </si>
+  <si>
+    <t>Folios Expedientes Marelli</t>
+  </si>
+  <si>
+    <t>Lunes a Domingo del día anterior</t>
+  </si>
+  <si>
+    <t>Ftp,zip,  pdf,xml, correo,excel</t>
+  </si>
+  <si>
+    <t>Control Digitalizacion3</t>
+  </si>
+  <si>
+    <t>Lunes a Sábado</t>
+  </si>
+  <si>
+    <t>VACIO</t>
+  </si>
+  <si>
+    <t>Lunes a Domingo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PENDIENTE DE RECIBIR </t>
+  </si>
+  <si>
+    <t>Facturas Pendientes en cedis ori</t>
+  </si>
+  <si>
+    <t>Lunes a Viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusion Pendientes CD LTL y Picking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRECTO </t>
+  </si>
+  <si>
+    <t>Lista de citas</t>
+  </si>
+  <si>
+    <t>CORRECTO 06:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAF Fondo Fijo Empresa 29 MXN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunes a Viernes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logis GSK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entregas Logis-Fuji </t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>procedimientos</t>
+  </si>
+  <si>
+    <t>AICM</t>
+  </si>
+  <si>
+    <t>SMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Día 1 y/o 2 de cada Mes (100 notif. Aprox en 2 bloques) </t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Día vencido laboral diario</t>
+  </si>
+  <si>
+    <t>Los miércoles con información de la semana anterior</t>
+  </si>
+  <si>
+    <t>Complejidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5295,8 +5462,75 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5309,8 +5543,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -5361,11 +5619,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5393,6 +5662,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5710,7 +6041,7 @@
   <dimension ref="A1:R1347"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6529,7 +6860,9 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="M21" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N21" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10051,8 +10384,8 @@
       <c r="D105" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E105" s="5" t="s">
-        <v>1101</v>
+      <c r="E105" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
@@ -10061,23 +10394,17 @@
         <v>1679</v>
       </c>
       <c r="J105" s="8"/>
-      <c r="K105" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L105" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M105" s="8"/>
+      <c r="K105" s="8"/>
+      <c r="L105" s="8"/>
+      <c r="M105" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N105" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O105" s="8"/>
-      <c r="P105" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q105" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P105" s="8"/>
+      <c r="Q105" s="8"/>
       <c r="R105" s="8"/>
     </row>
     <row r="106" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10093,8 +10420,8 @@
       <c r="D106" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E106" s="5" t="s">
-        <v>1101</v>
+      <c r="E106" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5" t="s">
@@ -10105,23 +10432,17 @@
         <v>1679</v>
       </c>
       <c r="J106" s="8"/>
-      <c r="K106" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L106" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M106" s="8"/>
+      <c r="K106" s="8"/>
+      <c r="L106" s="8"/>
+      <c r="M106" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N106" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O106" s="8"/>
-      <c r="P106" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q106" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P106" s="8"/>
+      <c r="Q106" s="8"/>
       <c r="R106" s="8"/>
     </row>
     <row r="107" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10137,8 +10458,8 @@
       <c r="D107" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E107" s="5" t="s">
-        <v>1101</v>
+      <c r="E107" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F107" s="5"/>
       <c r="G107" s="5" t="s">
@@ -10149,23 +10470,17 @@
         <v>1679</v>
       </c>
       <c r="J107" s="8"/>
-      <c r="K107" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L107" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M107" s="8"/>
+      <c r="K107" s="8"/>
+      <c r="L107" s="8"/>
+      <c r="M107" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N107" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O107" s="8"/>
-      <c r="P107" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q107" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P107" s="8"/>
+      <c r="Q107" s="8"/>
       <c r="R107" s="8"/>
     </row>
     <row r="108" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10181,8 +10496,8 @@
       <c r="D108" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E108" s="5" t="s">
-        <v>1101</v>
+      <c r="E108" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F108" s="5"/>
       <c r="G108" s="5" t="s">
@@ -10193,23 +10508,17 @@
         <v>1679</v>
       </c>
       <c r="J108" s="8"/>
-      <c r="K108" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L108" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M108" s="8"/>
+      <c r="K108" s="8"/>
+      <c r="L108" s="8"/>
+      <c r="M108" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N108" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O108" s="8"/>
-      <c r="P108" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q108" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P108" s="8"/>
+      <c r="Q108" s="8"/>
       <c r="R108" s="8"/>
     </row>
     <row r="109" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10225,8 +10534,8 @@
       <c r="D109" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E109" s="5" t="s">
-        <v>1101</v>
+      <c r="E109" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F109" s="5"/>
       <c r="G109" s="5" t="s">
@@ -10237,23 +10546,17 @@
         <v>1679</v>
       </c>
       <c r="J109" s="8"/>
-      <c r="K109" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L109" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M109" s="8"/>
+      <c r="K109" s="8"/>
+      <c r="L109" s="8"/>
+      <c r="M109" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N109" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O109" s="8"/>
-      <c r="P109" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q109" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P109" s="8"/>
+      <c r="Q109" s="8"/>
       <c r="R109" s="8"/>
     </row>
     <row r="110" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10269,8 +10572,8 @@
       <c r="D110" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E110" s="5" t="s">
-        <v>1101</v>
+      <c r="E110" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="5" t="s">
@@ -10281,23 +10584,17 @@
         <v>1679</v>
       </c>
       <c r="J110" s="8"/>
-      <c r="K110" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L110" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M110" s="8"/>
+      <c r="K110" s="8"/>
+      <c r="L110" s="8"/>
+      <c r="M110" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N110" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O110" s="8"/>
-      <c r="P110" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q110" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P110" s="8"/>
+      <c r="Q110" s="8"/>
       <c r="R110" s="8"/>
     </row>
     <row r="111" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10313,8 +10610,8 @@
       <c r="D111" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>1101</v>
+      <c r="E111" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F111" s="5"/>
       <c r="G111" s="5" t="s">
@@ -10325,23 +10622,17 @@
         <v>1679</v>
       </c>
       <c r="J111" s="8"/>
-      <c r="K111" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L111" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M111" s="8"/>
+      <c r="K111" s="8"/>
+      <c r="L111" s="8"/>
+      <c r="M111" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N111" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O111" s="8"/>
-      <c r="P111" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q111" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P111" s="8"/>
+      <c r="Q111" s="8"/>
       <c r="R111" s="8"/>
     </row>
     <row r="112" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10357,8 +10648,8 @@
       <c r="D112" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E112" s="5" t="s">
-        <v>1101</v>
+      <c r="E112" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F112" s="5"/>
       <c r="G112" s="5" t="s">
@@ -10369,23 +10660,17 @@
         <v>1679</v>
       </c>
       <c r="J112" s="8"/>
-      <c r="K112" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L112" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M112" s="8"/>
+      <c r="K112" s="8"/>
+      <c r="L112" s="8"/>
+      <c r="M112" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N112" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O112" s="8"/>
-      <c r="P112" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q112" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P112" s="8"/>
+      <c r="Q112" s="8"/>
       <c r="R112" s="8"/>
     </row>
     <row r="113" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10401,8 +10686,8 @@
       <c r="D113" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E113" s="5" t="s">
-        <v>1101</v>
+      <c r="E113" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F113" s="5"/>
       <c r="G113" s="5" t="s">
@@ -10413,23 +10698,17 @@
         <v>1679</v>
       </c>
       <c r="J113" s="8"/>
-      <c r="K113" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L113" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M113" s="8"/>
+      <c r="K113" s="8"/>
+      <c r="L113" s="8"/>
+      <c r="M113" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N113" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O113" s="8"/>
-      <c r="P113" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q113" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P113" s="8"/>
+      <c r="Q113" s="8"/>
       <c r="R113" s="8"/>
     </row>
     <row r="114" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10445,8 +10724,8 @@
       <c r="D114" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E114" s="5" t="s">
-        <v>1101</v>
+      <c r="E114" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="5" t="s">
@@ -10457,23 +10736,17 @@
         <v>1679</v>
       </c>
       <c r="J114" s="8"/>
-      <c r="K114" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L114" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M114" s="8"/>
+      <c r="K114" s="8"/>
+      <c r="L114" s="8"/>
+      <c r="M114" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N114" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O114" s="8"/>
-      <c r="P114" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q114" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P114" s="8"/>
+      <c r="Q114" s="8"/>
       <c r="R114" s="8"/>
     </row>
     <row r="115" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10489,8 +10762,8 @@
       <c r="D115" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E115" s="5" t="s">
-        <v>1101</v>
+      <c r="E115" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="5" t="s">
@@ -10501,23 +10774,17 @@
         <v>1679</v>
       </c>
       <c r="J115" s="8"/>
-      <c r="K115" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L115" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M115" s="8"/>
+      <c r="K115" s="8"/>
+      <c r="L115" s="8"/>
+      <c r="M115" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N115" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O115" s="8"/>
-      <c r="P115" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q115" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P115" s="8"/>
+      <c r="Q115" s="8"/>
       <c r="R115" s="8"/>
     </row>
     <row r="116" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
@@ -10533,8 +10800,8 @@
       <c r="D116" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E116" s="5" t="s">
-        <v>1101</v>
+      <c r="E116" s="9" t="s">
+        <v>1682</v>
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="5" t="s">
@@ -10545,23 +10812,17 @@
         <v>1679</v>
       </c>
       <c r="J116" s="8"/>
-      <c r="K116" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L116" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="M116" s="8"/>
+      <c r="K116" s="8"/>
+      <c r="L116" s="8"/>
+      <c r="M116" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N116" s="8" t="s">
         <v>1679</v>
       </c>
       <c r="O116" s="8"/>
-      <c r="P116" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q116" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P116" s="8"/>
+      <c r="Q116" s="8"/>
       <c r="R116" s="8"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
@@ -10578,7 +10839,7 @@
         <v>4</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
@@ -10589,7 +10850,9 @@
       <c r="J117" s="8"/>
       <c r="K117" s="8"/>
       <c r="L117" s="8"/>
-      <c r="M117" s="8"/>
+      <c r="M117" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N117" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10612,7 +10875,7 @@
         <v>4</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5" t="s">
@@ -10625,7 +10888,9 @@
       <c r="J118" s="8"/>
       <c r="K118" s="8"/>
       <c r="L118" s="8"/>
-      <c r="M118" s="8"/>
+      <c r="M118" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N118" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10634,7 +10899,7 @@
       <c r="Q118" s="8"/>
       <c r="R118" s="8"/>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>17</v>
       </c>
@@ -10648,7 +10913,7 @@
         <v>4</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F119" s="5"/>
       <c r="G119" s="5" t="s">
@@ -10661,7 +10926,9 @@
       <c r="J119" s="8"/>
       <c r="K119" s="8"/>
       <c r="L119" s="8"/>
-      <c r="M119" s="8"/>
+      <c r="M119" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N119" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10670,7 +10937,7 @@
       <c r="Q119" s="8"/>
       <c r="R119" s="8"/>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>17</v>
       </c>
@@ -10684,7 +10951,7 @@
         <v>4</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="5" t="s">
@@ -10697,7 +10964,9 @@
       <c r="J120" s="8"/>
       <c r="K120" s="8"/>
       <c r="L120" s="8"/>
-      <c r="M120" s="8"/>
+      <c r="M120" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N120" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10706,7 +10975,7 @@
       <c r="Q120" s="8"/>
       <c r="R120" s="8"/>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>17</v>
       </c>
@@ -10720,7 +10989,7 @@
         <v>4</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="5" t="s">
@@ -10733,7 +11002,9 @@
       <c r="J121" s="8"/>
       <c r="K121" s="8"/>
       <c r="L121" s="8"/>
-      <c r="M121" s="8"/>
+      <c r="M121" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N121" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10742,7 +11013,7 @@
       <c r="Q121" s="8"/>
       <c r="R121" s="8"/>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>17</v>
       </c>
@@ -10756,7 +11027,7 @@
         <v>4</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F122" s="5"/>
       <c r="G122" s="5" t="s">
@@ -10769,7 +11040,9 @@
       <c r="J122" s="8"/>
       <c r="K122" s="8"/>
       <c r="L122" s="8"/>
-      <c r="M122" s="8"/>
+      <c r="M122" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N122" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10778,7 +11051,7 @@
       <c r="Q122" s="8"/>
       <c r="R122" s="8"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>17</v>
       </c>
@@ -10792,7 +11065,7 @@
         <v>4</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F123" s="5"/>
       <c r="G123" s="5" t="s">
@@ -10805,7 +11078,9 @@
       <c r="J123" s="8"/>
       <c r="K123" s="8"/>
       <c r="L123" s="8"/>
-      <c r="M123" s="8"/>
+      <c r="M123" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N123" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10828,7 +11103,7 @@
         <v>4</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F124" s="5"/>
       <c r="G124" s="5" t="s">
@@ -10841,7 +11116,9 @@
       <c r="J124" s="8"/>
       <c r="K124" s="8"/>
       <c r="L124" s="8"/>
-      <c r="M124" s="8"/>
+      <c r="M124" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N124" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10864,7 +11141,7 @@
         <v>4</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F125" s="5"/>
       <c r="G125" s="5" t="s">
@@ -10877,7 +11154,9 @@
       <c r="J125" s="8"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8"/>
-      <c r="M125" s="8"/>
+      <c r="M125" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N125" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10900,7 +11179,7 @@
         <v>4</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F126" s="5"/>
       <c r="G126" s="5" t="s">
@@ -10913,7 +11192,9 @@
       <c r="J126" s="8"/>
       <c r="K126" s="8"/>
       <c r="L126" s="8"/>
-      <c r="M126" s="8"/>
+      <c r="M126" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N126" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10936,7 +11217,7 @@
         <v>4</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F127" s="5"/>
       <c r="G127" s="5" t="s">
@@ -10949,7 +11230,9 @@
       <c r="J127" s="8"/>
       <c r="K127" s="8"/>
       <c r="L127" s="8"/>
-      <c r="M127" s="8"/>
+      <c r="M127" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N127" s="8" t="s">
         <v>1679</v>
       </c>
@@ -10972,7 +11255,7 @@
         <v>4</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F128" s="5"/>
       <c r="G128" s="5" t="s">
@@ -10985,7 +11268,9 @@
       <c r="J128" s="8"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8"/>
-      <c r="M128" s="8"/>
+      <c r="M128" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N128" s="8" t="s">
         <v>1679</v>
       </c>
@@ -11008,7 +11293,7 @@
         <v>4</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F129" s="5"/>
       <c r="G129" s="5" t="s">
@@ -11021,7 +11306,9 @@
       <c r="J129" s="8"/>
       <c r="K129" s="8"/>
       <c r="L129" s="8"/>
-      <c r="M129" s="8"/>
+      <c r="M129" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N129" s="8" t="s">
         <v>1679</v>
       </c>
@@ -11044,7 +11331,7 @@
         <v>4</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F130" s="9"/>
       <c r="G130" s="9" t="s">
@@ -11057,7 +11344,9 @@
       <c r="J130" s="8"/>
       <c r="K130" s="8"/>
       <c r="L130" s="8"/>
-      <c r="M130" s="8"/>
+      <c r="M130" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N130" s="8" t="s">
         <v>1679</v>
       </c>
@@ -11080,7 +11369,7 @@
         <v>4</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F131" s="5"/>
       <c r="G131" s="5" t="s">
@@ -11093,7 +11382,9 @@
       <c r="J131" s="8"/>
       <c r="K131" s="8"/>
       <c r="L131" s="8"/>
-      <c r="M131" s="8"/>
+      <c r="M131" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N131" s="8" t="s">
         <v>1679</v>
       </c>
@@ -11116,7 +11407,7 @@
         <v>4</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>1090</v>
+        <v>1684</v>
       </c>
       <c r="F132" s="9"/>
       <c r="G132" s="9" t="s">
@@ -11129,7 +11420,9 @@
       <c r="J132" s="8"/>
       <c r="K132" s="8"/>
       <c r="L132" s="8"/>
-      <c r="M132" s="8"/>
+      <c r="M132" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N132" s="8" t="s">
         <v>1679</v>
       </c>
@@ -14392,7 +14685,7 @@
       </c>
       <c r="D224" s="5"/>
       <c r="E224" s="5" t="s">
-        <v>1090</v>
+        <v>1681</v>
       </c>
       <c r="F224" s="5"/>
       <c r="G224" s="5"/>
@@ -14403,7 +14696,9 @@
       <c r="J224" s="8"/>
       <c r="K224" s="8"/>
       <c r="L224" s="8"/>
-      <c r="M224" s="8"/>
+      <c r="M224" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N224" s="8" t="s">
         <v>1679</v>
       </c>
@@ -14478,7 +14773,7 @@
       <c r="Q226" s="8"/>
       <c r="R226" s="8"/>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>39</v>
       </c>
@@ -14890,7 +15185,7 @@
       </c>
       <c r="D238" s="5"/>
       <c r="E238" s="5" t="s">
-        <v>1090</v>
+        <v>1681</v>
       </c>
       <c r="F238" s="5"/>
       <c r="G238" s="5"/>
@@ -14901,7 +15196,9 @@
       <c r="J238" s="8"/>
       <c r="K238" s="8"/>
       <c r="L238" s="8"/>
-      <c r="M238" s="8"/>
+      <c r="M238" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N238" s="8" t="s">
         <v>1679</v>
       </c>
@@ -14922,7 +15219,7 @@
       </c>
       <c r="D239" s="5"/>
       <c r="E239" s="5" t="s">
-        <v>1090</v>
+        <v>1681</v>
       </c>
       <c r="F239" s="5"/>
       <c r="G239" s="5"/>
@@ -14933,7 +15230,9 @@
       <c r="J239" s="8"/>
       <c r="K239" s="8"/>
       <c r="L239" s="8"/>
-      <c r="M239" s="8"/>
+      <c r="M239" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N239" s="8" t="s">
         <v>1679</v>
       </c>
@@ -14990,7 +15289,7 @@
       </c>
       <c r="D241" s="5"/>
       <c r="E241" s="5" t="s">
-        <v>1690</v>
+        <v>1684</v>
       </c>
       <c r="F241" s="5"/>
       <c r="G241" s="5"/>
@@ -14999,14 +15298,14 @@
         <v>1679</v>
       </c>
       <c r="J241" s="8"/>
-      <c r="K241" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="K241" s="8"/>
       <c r="L241" s="8"/>
       <c r="M241" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="N241" s="8"/>
+      <c r="N241" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="O241" s="8"/>
       <c r="P241" s="8"/>
       <c r="Q241" s="8"/>
@@ -15764,7 +16063,7 @@
       <c r="Q262" s="8"/>
       <c r="R262" s="8"/>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A263" s="5">
         <v>67</v>
       </c>
@@ -18106,7 +18405,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="324" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
         <v>102</v>
       </c>
@@ -19813,8 +20112,8 @@
       <c r="D368" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E368" s="5" t="s">
-        <v>1706</v>
+      <c r="E368" s="10" t="s">
+        <v>1681</v>
       </c>
       <c r="F368" s="5"/>
       <c r="G368" s="5"/>
@@ -19833,9 +20132,7 @@
       </c>
       <c r="O368" s="8"/>
       <c r="P368" s="8"/>
-      <c r="Q368" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="Q368" s="8"/>
       <c r="R368" s="8"/>
     </row>
     <row r="369" spans="1:18" x14ac:dyDescent="0.25">
@@ -19851,8 +20148,8 @@
       <c r="D369" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E369" s="5" t="s">
-        <v>1706</v>
+      <c r="E369" s="10" t="s">
+        <v>1681</v>
       </c>
       <c r="F369" s="5"/>
       <c r="G369" s="5" t="s">
@@ -19873,9 +20170,7 @@
       </c>
       <c r="O369" s="8"/>
       <c r="P369" s="8"/>
-      <c r="Q369" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="Q369" s="8"/>
       <c r="R369" s="8"/>
     </row>
     <row r="370" spans="1:18" x14ac:dyDescent="0.25">
@@ -21146,7 +21441,7 @@
       </c>
       <c r="R403" s="8"/>
     </row>
-    <row r="404" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
         <v>138</v>
       </c>
@@ -21992,7 +22287,7 @@
       </c>
       <c r="R426" s="8"/>
     </row>
-    <row r="427" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A427" s="5">
         <v>153</v>
       </c>
@@ -23260,7 +23555,7 @@
       </c>
       <c r="R459" s="8"/>
     </row>
-    <row r="460" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A460" s="5">
         <v>173</v>
       </c>
@@ -25944,7 +26239,7 @@
       </c>
       <c r="R520" s="8"/>
     </row>
-    <row r="521" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A521" s="5">
         <v>173</v>
       </c>
@@ -26736,7 +27031,7 @@
       </c>
       <c r="R538" s="8"/>
     </row>
-    <row r="539" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A539" s="5">
         <v>173</v>
       </c>
@@ -33236,7 +33531,7 @@
       </c>
       <c r="R688" s="8"/>
     </row>
-    <row r="689" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A689" s="5">
         <v>174</v>
       </c>
@@ -40290,7 +40585,7 @@
         <v>4</v>
       </c>
       <c r="E867" s="5" t="s">
-        <v>1060</v>
+        <v>1684</v>
       </c>
       <c r="F867" s="9"/>
       <c r="G867" s="9"/>
@@ -41796,7 +42091,7 @@
       <c r="Q907" s="8"/>
       <c r="R907" s="8"/>
     </row>
-    <row r="908" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A908" s="5">
         <v>216</v>
       </c>
@@ -47652,7 +47947,7 @@
       </c>
       <c r="R1052" s="8"/>
     </row>
-    <row r="1053" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1053" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1053" s="10">
         <v>244</v>
       </c>
@@ -49794,7 +50089,7 @@
       </c>
       <c r="R1103" s="8"/>
     </row>
-    <row r="1104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1104" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1104" s="10">
         <v>244</v>
       </c>
@@ -53704,7 +53999,7 @@
         <v>4</v>
       </c>
       <c r="E1208" s="8" t="s">
-        <v>1693</v>
+        <v>1760</v>
       </c>
       <c r="F1208" s="8"/>
       <c r="G1208" s="8" t="s">
@@ -53723,8 +54018,12 @@
       <c r="N1208" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1208" s="8"/>
-      <c r="P1208" s="8"/>
+      <c r="O1208" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1208" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1208" s="8"/>
       <c r="R1208" s="8"/>
     </row>
@@ -53741,8 +54040,8 @@
       <c r="D1209" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1209" s="10" t="s">
-        <v>1693</v>
+      <c r="E1209" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1209" s="8"/>
       <c r="G1209" s="8" t="s">
@@ -53761,8 +54060,12 @@
       <c r="N1209" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1209" s="8"/>
-      <c r="P1209" s="8"/>
+      <c r="O1209" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1209" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1209" s="8"/>
       <c r="R1209" s="8"/>
     </row>
@@ -53779,8 +54082,8 @@
       <c r="D1210" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1210" s="10" t="s">
-        <v>1693</v>
+      <c r="E1210" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1210" s="10"/>
       <c r="G1210" s="10" t="s">
@@ -53799,8 +54102,12 @@
       <c r="N1210" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1210" s="8"/>
-      <c r="P1210" s="8"/>
+      <c r="O1210" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1210" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1210" s="8"/>
       <c r="R1210" s="8"/>
     </row>
@@ -53817,8 +54124,8 @@
       <c r="D1211" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1211" s="10" t="s">
-        <v>1693</v>
+      <c r="E1211" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1211" s="8"/>
       <c r="G1211" s="8" t="s">
@@ -53837,8 +54144,12 @@
       <c r="N1211" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1211" s="8"/>
-      <c r="P1211" s="8"/>
+      <c r="O1211" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1211" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1211" s="8"/>
       <c r="R1211" s="8"/>
     </row>
@@ -53855,8 +54166,8 @@
       <c r="D1212" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1212" s="10" t="s">
-        <v>1693</v>
+      <c r="E1212" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1212" s="10"/>
       <c r="G1212" s="10" t="s">
@@ -53875,8 +54186,12 @@
       <c r="N1212" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1212" s="8"/>
-      <c r="P1212" s="8"/>
+      <c r="O1212" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1212" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1212" s="8"/>
       <c r="R1212" s="8"/>
     </row>
@@ -53893,8 +54208,8 @@
       <c r="D1213" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1213" s="10" t="s">
-        <v>1693</v>
+      <c r="E1213" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1213" s="10"/>
       <c r="G1213" s="10" t="s">
@@ -53913,8 +54228,12 @@
       <c r="N1213" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1213" s="8"/>
-      <c r="P1213" s="8"/>
+      <c r="O1213" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1213" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1213" s="8"/>
       <c r="R1213" s="8"/>
     </row>
@@ -53932,7 +54251,7 @@
         <v>4</v>
       </c>
       <c r="E1214" s="8" t="s">
-        <v>1693</v>
+        <v>1760</v>
       </c>
       <c r="F1214" s="8"/>
       <c r="G1214" s="8" t="s">
@@ -53951,8 +54270,12 @@
       <c r="N1214" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1214" s="8"/>
-      <c r="P1214" s="8"/>
+      <c r="O1214" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1214" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1214" s="8"/>
       <c r="R1214" s="8"/>
     </row>
@@ -53970,7 +54293,7 @@
         <v>4</v>
       </c>
       <c r="E1215" s="8" t="s">
-        <v>1693</v>
+        <v>1760</v>
       </c>
       <c r="F1215" s="8"/>
       <c r="G1215" s="8" t="s">
@@ -53989,8 +54312,12 @@
       <c r="N1215" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1215" s="8"/>
-      <c r="P1215" s="8"/>
+      <c r="O1215" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1215" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1215" s="8"/>
       <c r="R1215" s="8"/>
     </row>
@@ -54008,7 +54335,7 @@
         <v>4</v>
       </c>
       <c r="E1216" s="8" t="s">
-        <v>1693</v>
+        <v>1760</v>
       </c>
       <c r="F1216" s="8"/>
       <c r="G1216" s="8" t="s">
@@ -54027,8 +54354,12 @@
       <c r="N1216" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1216" s="8"/>
-      <c r="P1216" s="8"/>
+      <c r="O1216" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1216" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1216" s="8"/>
       <c r="R1216" s="8"/>
     </row>
@@ -54045,8 +54376,8 @@
       <c r="D1217" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1217" s="10" t="s">
-        <v>1693</v>
+      <c r="E1217" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1217" s="10"/>
       <c r="G1217" s="10" t="s">
@@ -54065,8 +54396,12 @@
       <c r="N1217" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1217" s="8"/>
-      <c r="P1217" s="8"/>
+      <c r="O1217" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1217" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1217" s="8"/>
       <c r="R1217" s="8"/>
     </row>
@@ -54083,8 +54418,8 @@
       <c r="D1218" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1218" s="10" t="s">
-        <v>1693</v>
+      <c r="E1218" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1218" s="10"/>
       <c r="G1218" s="10" t="s">
@@ -54103,8 +54438,12 @@
       <c r="N1218" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1218" s="8"/>
-      <c r="P1218" s="8"/>
+      <c r="O1218" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1218" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1218" s="8"/>
       <c r="R1218" s="8"/>
     </row>
@@ -54121,8 +54460,8 @@
       <c r="D1219" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1219" s="10" t="s">
-        <v>1693</v>
+      <c r="E1219" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1219" s="10"/>
       <c r="G1219" s="10" t="s">
@@ -54141,8 +54480,12 @@
       <c r="N1219" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1219" s="8"/>
-      <c r="P1219" s="8"/>
+      <c r="O1219" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1219" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1219" s="8"/>
       <c r="R1219" s="8"/>
     </row>
@@ -54159,8 +54502,8 @@
       <c r="D1220" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1220" s="10" t="s">
-        <v>1693</v>
+      <c r="E1220" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1220" s="10"/>
       <c r="G1220" s="10" t="s">
@@ -54179,8 +54522,12 @@
       <c r="N1220" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1220" s="8"/>
-      <c r="P1220" s="8"/>
+      <c r="O1220" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1220" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1220" s="8"/>
       <c r="R1220" s="8"/>
     </row>
@@ -54197,8 +54544,8 @@
       <c r="D1221" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1221" s="10" t="s">
-        <v>1693</v>
+      <c r="E1221" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1221" s="10"/>
       <c r="G1221" s="10" t="s">
@@ -54217,8 +54564,12 @@
       <c r="N1221" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1221" s="8"/>
-      <c r="P1221" s="8"/>
+      <c r="O1221" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1221" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1221" s="8"/>
       <c r="R1221" s="8"/>
     </row>
@@ -54235,8 +54586,8 @@
       <c r="D1222" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1222" s="10" t="s">
-        <v>1693</v>
+      <c r="E1222" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1222" s="10"/>
       <c r="G1222" s="10" t="s">
@@ -54255,8 +54606,12 @@
       <c r="N1222" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1222" s="8"/>
-      <c r="P1222" s="8"/>
+      <c r="O1222" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1222" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1222" s="8"/>
       <c r="R1222" s="8"/>
     </row>
@@ -54273,8 +54628,8 @@
       <c r="D1223" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1223" s="10" t="s">
-        <v>1693</v>
+      <c r="E1223" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1223" s="10"/>
       <c r="G1223" s="10"/>
@@ -54291,8 +54646,12 @@
       <c r="N1223" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1223" s="8"/>
-      <c r="P1223" s="8"/>
+      <c r="O1223" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1223" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1223" s="8"/>
       <c r="R1223" s="8"/>
     </row>
@@ -54309,8 +54668,8 @@
       <c r="D1224" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1224" s="10" t="s">
-        <v>1693</v>
+      <c r="E1224" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1224" s="10"/>
       <c r="G1224" s="10" t="s">
@@ -54329,8 +54688,12 @@
       <c r="N1224" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1224" s="8"/>
-      <c r="P1224" s="8"/>
+      <c r="O1224" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1224" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1224" s="8"/>
       <c r="R1224" s="8"/>
     </row>
@@ -54347,8 +54710,8 @@
       <c r="D1225" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1225" s="10" t="s">
-        <v>1693</v>
+      <c r="E1225" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1225" s="10"/>
       <c r="G1225" s="10" t="s">
@@ -54367,8 +54730,12 @@
       <c r="N1225" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1225" s="8"/>
-      <c r="P1225" s="8"/>
+      <c r="O1225" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1225" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1225" s="8"/>
       <c r="R1225" s="8"/>
     </row>
@@ -54385,8 +54752,8 @@
       <c r="D1226" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1226" s="10" t="s">
-        <v>1693</v>
+      <c r="E1226" s="8" t="s">
+        <v>1760</v>
       </c>
       <c r="F1226" s="10"/>
       <c r="G1226" s="10" t="s">
@@ -54405,8 +54772,12 @@
       <c r="N1226" s="8" t="s">
         <v>1679</v>
       </c>
-      <c r="O1226" s="8"/>
-      <c r="P1226" s="8"/>
+      <c r="O1226" s="8" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P1226" s="11" t="s">
+        <v>1679</v>
+      </c>
       <c r="Q1226" s="8"/>
       <c r="R1226" s="8"/>
     </row>
@@ -55946,7 +56317,7 @@
       <c r="Q1263" s="8"/>
       <c r="R1263" s="8"/>
     </row>
-    <row r="1264" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1264" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1264" s="10">
         <v>322</v>
       </c>
@@ -57511,8 +57882,8 @@
       <c r="D1305" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1305" s="8" t="s">
-        <v>1696</v>
+      <c r="E1305" s="10" t="s">
+        <v>1684</v>
       </c>
       <c r="F1305" s="8"/>
       <c r="G1305" s="8"/>
@@ -57521,12 +57892,8 @@
         <v>1679</v>
       </c>
       <c r="J1305" s="8"/>
-      <c r="K1305" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L1305" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="K1305" s="8"/>
+      <c r="L1305" s="8"/>
       <c r="M1305" s="8" t="s">
         <v>1679</v>
       </c>
@@ -57534,12 +57901,8 @@
         <v>1679</v>
       </c>
       <c r="O1305" s="8"/>
-      <c r="P1305" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q1305" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P1305" s="8"/>
+      <c r="Q1305" s="8"/>
       <c r="R1305" s="8"/>
     </row>
     <row r="1306" spans="1:18" x14ac:dyDescent="0.25">
@@ -57556,7 +57919,7 @@
         <v>4</v>
       </c>
       <c r="E1306" s="10" t="s">
-        <v>1696</v>
+        <v>1684</v>
       </c>
       <c r="F1306" s="8"/>
       <c r="G1306" s="8" t="s">
@@ -57567,12 +57930,8 @@
         <v>1679</v>
       </c>
       <c r="J1306" s="8"/>
-      <c r="K1306" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="L1306" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="K1306" s="8"/>
+      <c r="L1306" s="8"/>
       <c r="M1306" s="8" t="s">
         <v>1679</v>
       </c>
@@ -57580,12 +57939,8 @@
         <v>1679</v>
       </c>
       <c r="O1306" s="8"/>
-      <c r="P1306" s="8" t="s">
-        <v>1679</v>
-      </c>
-      <c r="Q1306" s="8" t="s">
-        <v>1679</v>
-      </c>
+      <c r="P1306" s="8"/>
+      <c r="Q1306" s="8"/>
       <c r="R1306" s="8"/>
     </row>
     <row r="1307" spans="1:18" x14ac:dyDescent="0.25">
@@ -58124,7 +58479,7 @@
       <c r="Q1320" s="8"/>
       <c r="R1320" s="8"/>
     </row>
-    <row r="1321" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1321" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1321" s="10">
         <v>334</v>
       </c>
@@ -58166,7 +58521,7 @@
       <c r="Q1321" s="8"/>
       <c r="R1321" s="8"/>
     </row>
-    <row r="1322" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1322" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1322" s="10">
         <v>334</v>
       </c>
@@ -58208,7 +58563,7 @@
       <c r="Q1322" s="8"/>
       <c r="R1322" s="8"/>
     </row>
-    <row r="1323" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1323" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1323" s="10">
         <v>334</v>
       </c>
@@ -58250,7 +58605,7 @@
       <c r="Q1323" s="8"/>
       <c r="R1323" s="8"/>
     </row>
-    <row r="1324" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1324" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1324" s="10">
         <v>334</v>
       </c>
@@ -58424,7 +58779,7 @@
         <v>4</v>
       </c>
       <c r="E1328" s="10" t="s">
-        <v>1072</v>
+        <v>1719</v>
       </c>
       <c r="F1328" s="10"/>
       <c r="G1328" s="10"/>
@@ -58435,7 +58790,9 @@
       <c r="J1328" s="8"/>
       <c r="K1328" s="8"/>
       <c r="L1328" s="8"/>
-      <c r="M1328" s="8"/>
+      <c r="M1328" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N1328" s="8" t="s">
         <v>1679</v>
       </c>
@@ -58458,7 +58815,7 @@
         <v>4</v>
       </c>
       <c r="E1329" s="10" t="s">
-        <v>1072</v>
+        <v>1719</v>
       </c>
       <c r="F1329" s="10"/>
       <c r="G1329" s="10" t="s">
@@ -58471,7 +58828,9 @@
       <c r="J1329" s="8"/>
       <c r="K1329" s="8"/>
       <c r="L1329" s="8"/>
-      <c r="M1329" s="8"/>
+      <c r="M1329" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N1329" s="8" t="s">
         <v>1679</v>
       </c>
@@ -58494,7 +58853,7 @@
         <v>5</v>
       </c>
       <c r="E1330" s="10" t="s">
-        <v>1072</v>
+        <v>1682</v>
       </c>
       <c r="F1330" s="8"/>
       <c r="G1330" s="8"/>
@@ -58505,7 +58864,9 @@
       <c r="J1330" s="8"/>
       <c r="K1330" s="8"/>
       <c r="L1330" s="8"/>
-      <c r="M1330" s="8"/>
+      <c r="M1330" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N1330" s="8" t="s">
         <v>1679</v>
       </c>
@@ -58528,7 +58889,7 @@
         <v>5</v>
       </c>
       <c r="E1331" s="10" t="s">
-        <v>1072</v>
+        <v>1719</v>
       </c>
       <c r="F1331" s="10"/>
       <c r="G1331" s="10" t="s">
@@ -58541,7 +58902,9 @@
       <c r="J1331" s="8"/>
       <c r="K1331" s="8"/>
       <c r="L1331" s="8"/>
-      <c r="M1331" s="8"/>
+      <c r="M1331" s="8" t="s">
+        <v>1679</v>
+      </c>
       <c r="N1331" s="8" t="s">
         <v>1679</v>
       </c>
@@ -59145,4 +59508,790 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>1783</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>1784</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>1787</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>1776</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>1708</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1</v>
+      </c>
+      <c r="I2" s="12">
+        <v>3</v>
+      </c>
+      <c r="J2" s="12">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>1684</v>
+      </c>
+      <c r="H3" s="12">
+        <v>2</v>
+      </c>
+      <c r="I3" s="12">
+        <v>2</v>
+      </c>
+      <c r="J3" s="12">
+        <f>3+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>1684</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2</v>
+      </c>
+      <c r="J4" s="12">
+        <f>4+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="19" t="s">
+        <v>1772</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>1684</v>
+      </c>
+      <c r="H5" s="12">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12">
+        <f>4+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="19" t="s">
+        <v>1774</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>2</v>
+      </c>
+      <c r="J6" s="12">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="21" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>1726</v>
+      </c>
+      <c r="H8" s="12">
+        <v>7</v>
+      </c>
+      <c r="I8" s="12">
+        <v>5</v>
+      </c>
+      <c r="J8" s="12">
+        <f>4+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>1786</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>1716</v>
+      </c>
+      <c r="H9" s="12">
+        <v>8</v>
+      </c>
+      <c r="I9" s="12">
+        <v>10</v>
+      </c>
+      <c r="J9" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>1786</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>1716</v>
+      </c>
+      <c r="H10" s="12">
+        <v>8</v>
+      </c>
+      <c r="I10" s="12">
+        <v>10</v>
+      </c>
+      <c r="J10" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H11" s="12">
+        <v>9</v>
+      </c>
+      <c r="I11" s="12">
+        <v>9</v>
+      </c>
+      <c r="J11" s="12">
+        <f>4+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="19" t="s">
+        <v>1768</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H12" s="12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="12">
+        <v>13</v>
+      </c>
+      <c r="J12" s="12">
+        <f>6+7</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H13" s="12">
+        <v>11</v>
+      </c>
+      <c r="I13" s="12">
+        <v>2</v>
+      </c>
+      <c r="J13" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="19" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>1707</v>
+      </c>
+      <c r="H14" s="12">
+        <v>12</v>
+      </c>
+      <c r="I14" s="12">
+        <v>5</v>
+      </c>
+      <c r="J14" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="19" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H15" s="12">
+        <v>13</v>
+      </c>
+      <c r="I15" s="12">
+        <v>4</v>
+      </c>
+      <c r="J15" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="19" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>1690</v>
+      </c>
+      <c r="H16" s="12">
+        <v>14</v>
+      </c>
+      <c r="I16" s="12">
+        <v>11</v>
+      </c>
+      <c r="J16" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="19" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>1762</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>1725</v>
+      </c>
+      <c r="H17" s="12">
+        <v>15</v>
+      </c>
+      <c r="I17" s="12">
+        <v>12</v>
+      </c>
+      <c r="J17" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>1696</v>
+      </c>
+      <c r="H18" s="12">
+        <v>16</v>
+      </c>
+      <c r="I18" s="12">
+        <v>12</v>
+      </c>
+      <c r="J18" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="19" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H19" s="12">
+        <v>17</v>
+      </c>
+      <c r="I19" s="12">
+        <v>29</v>
+      </c>
+      <c r="J19" s="12">
+        <f>15+5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>1684</v>
+      </c>
+      <c r="H20" s="12">
+        <v>18</v>
+      </c>
+      <c r="I20" s="12">
+        <v>32</v>
+      </c>
+      <c r="J20" s="28">
+        <f>5+2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="H21" s="12">
+        <v>19</v>
+      </c>
+      <c r="I21" s="12">
+        <v>35</v>
+      </c>
+      <c r="J21" s="12">
+        <f>3+8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="19" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>1681</v>
+      </c>
+      <c r="H22" s="12">
+        <v>20</v>
+      </c>
+      <c r="I22" s="12">
+        <v>61</v>
+      </c>
+      <c r="J22" s="12">
+        <f>9+2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="19" t="s">
+        <v>1622</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H23" s="12">
+        <v>21</v>
+      </c>
+      <c r="I23" s="12">
+        <v>76</v>
+      </c>
+      <c r="J23" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>1760</v>
+      </c>
+      <c r="H24" s="12">
+        <v>22</v>
+      </c>
+      <c r="I24" s="12">
+        <v>78</v>
+      </c>
+      <c r="J24" s="12">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>